<commit_message>
Documentos finales grado 6 g 12
Documentos  finales después de corrección de estilo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion12/SolicitudGrafica_CN_06_12_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion12/SolicitudGrafica_CN_06_12_CO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="214">
   <si>
     <t>Fecha:</t>
   </si>
@@ -697,15 +697,42 @@
     <t>http://upload.wikimedia.org/wikipedia/commons/b/bb/GasDepositDiagram.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Traducir la imagen 
+    <t>Shutterstock 122566315</t>
+  </si>
+  <si>
+    <t>Planta nuclear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Por favor traducir los indicadores al español
+House Light : Luz de la casa
+Power lines: Cables de electricidad
+Dam: dique
+Reservoir: embalse
+Penstocks: conducto
+Intake y control gate: compuerta de admisión. Solo dejar una de las palabra inicadas
+Turbine: turbina
+Outflow: desagüe
+Power house:Central eléctrica
+Transformer: transformador
+Generator: generador
 </t>
   </si>
   <si>
-    <t>Shutterstock 122566315</t>
-  </si>
-  <si>
-    <t>Planta nuclear</t>
+    <t xml:space="preserve">Traducir:
+Absolute zero: cero absoluto
+The freezing point of wáter: punto de fusióndel agua
+The boiling point of water: punto de ebullición del agua
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No colocar el título
+Conventional non- assiciated gas: Pozos de gas aislados
+Land Surface: superficie de la tierra
+Coalbed methane: Metano en capas de carbón
+Conventional assiciated gas: Pozos de gas
+Tight sand gas: gas atrapado en la arena
+Gas rich shale: gas de lutita
+</t>
   </si>
 </sst>
 </file>
@@ -2454,15 +2481,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1973035</xdr:colOff>
+      <xdr:colOff>3605892</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>217714</xdr:rowOff>
+      <xdr:rowOff>149680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3754210</xdr:colOff>
+      <xdr:colOff>5387067</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>2769779</xdr:rowOff>
+      <xdr:rowOff>2701745</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2484,7 +2511,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="18600964" y="26452285"/>
+          <a:off x="19281321" y="28738287"/>
           <a:ext cx="1781175" cy="2552065"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2865,15 +2892,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1687286</xdr:colOff>
+      <xdr:colOff>3088821</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>204107</xdr:rowOff>
+      <xdr:rowOff>272143</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>4553041</xdr:colOff>
+      <xdr:colOff>5592537</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>2091962</xdr:rowOff>
+      <xdr:rowOff>2068285</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2895,8 +2922,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="18315215" y="45202928"/>
-          <a:ext cx="2865755" cy="1887855"/>
+          <a:off x="18764250" y="47625000"/>
+          <a:ext cx="2503716" cy="1796142"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3576,9 +3603,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32:XFD46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4044,7 +4071,7 @@
       </c>
       <c r="K16" s="89"/>
     </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="12" customFormat="1" ht="345.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG08</v>
@@ -4081,7 +4108,9 @@
       <c r="J17" s="81" t="s">
         <v>178</v>
       </c>
-      <c r="K17" s="73"/>
+      <c r="K17" s="73" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="18" spans="1:11" s="12" customFormat="1" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="str">
@@ -4234,7 +4263,9 @@
       <c r="J21" s="95" t="s">
         <v>188</v>
       </c>
-      <c r="K21" s="92"/>
+      <c r="K21" s="92" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="22" spans="1:11" s="12" customFormat="1" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="74" t="s">
@@ -4577,7 +4608,7 @@
         <v>160</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="12" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4585,7 +4616,7 @@
         <v>205</v>
       </c>
       <c r="B31" s="88" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C31" s="25" t="str">
         <f t="shared" si="4"/>
@@ -4614,7 +4645,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K31" s="19"/>
     </row>

</xml_diff>